<commit_message>
integrate the annexe list in the HLM template
</commit_message>
<xml_diff>
--- a/static/files/annexes.xlsx
+++ b/static/files/annexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6020E-1AAB-5E45-BC33-604CA372B835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF2B7F7-F9F3-444C-BB79-5F173EBFBA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -44,9 +44,6 @@
     <t>1. Telechager le modèle (ce fichier)</t>
   </si>
   <si>
-    <t>2. Modifier à votre guise le fichier pour modifier la liste des prêts</t>
-  </si>
-  <si>
     <t>3. Enregistrer vos modifications</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>T5 et plus</t>
   </si>
   <si>
-    <t>si des logements sont déjà assignés à la convention, alors ils seront exportés dans le fichier modèle</t>
-  </si>
-  <si>
-    <t>5. Vérifier le contenu téléversé dans l'application et enrigistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
-  </si>
-  <si>
     <t>Désignation des logements</t>
   </si>
   <si>
@@ -105,6 +96,12 @@
   </si>
   <si>
     <t>Surface de l'annexe</t>
+  </si>
+  <si>
+    <t>2. Modifier à votre guise le fichier</t>
+  </si>
+  <si>
+    <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
   </si>
 </sst>
 </file>
@@ -694,22 +691,22 @@
   <sheetData>
     <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1154,11 +1151,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467F41B6-50A5-F34D-9811-537B9541F979}">
-  <dimension ref="B2:B10"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1178,7 +1173,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1193,21 +1188,16 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0IlGhDNZkMw1CpkJ22VrGnFOy5A1ba4VPUPDVGooSHmeI18rAH1D1+kQRd1kfaflIdffD1eeJO4DjXF1/JC4uA==" saltValue="z53X+BT+GWeylWBMFBybHQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="MU3KMvdpsWCrXPo+0vW46AToCNKDCtwVVWiPZE+SH16oHAk6QUXj0pCjoJcKe+MJtGPCbpv8OvQ0gcusU4fALQ==" saltValue="/FTo2cbFRX34J/jzXJaMLg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1226,44 +1216,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>